<commit_message>
Use total number of available bakcfill, not adjusted figures
</commit_message>
<xml_diff>
--- a/data/figure_3/Backfill consumption.xlsx
+++ b/data/figure_3/Backfill consumption.xlsx
@@ -504,7 +504,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{6F0310EE-1B88-8647-B861-0BEEBDCA64F8}</c15:txfldGUID>
+                      <c15:txfldGUID>{7C01827B-D930-8F46-87F4-AEBB7D0AA88B}</c15:txfldGUID>
                       <c15:f>Sheet1!$B$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -544,7 +544,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{78DCAE88-7126-E340-B3A0-C9CAB754A082}</c15:txfldGUID>
+                      <c15:txfldGUID>{BE9742D8-B4D1-AB45-8D7B-3C8DD49E7652}</c15:txfldGUID>
                       <c15:f>Sheet1!$C$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -584,7 +584,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{50F958D0-C664-014C-96CA-90813E43B59C}</c15:txfldGUID>
+                      <c15:txfldGUID>{8806F20C-38C8-774C-83FD-D9644622AD48}</c15:txfldGUID>
                       <c15:f>Sheet1!$D$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -624,7 +624,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{7BA246AE-7008-554C-82AB-0EC66CC74325}</c15:txfldGUID>
+                      <c15:txfldGUID>{E5E51F3F-36E7-1A41-A925-28B5F93EA2B4}</c15:txfldGUID>
                       <c15:f>Sheet1!$E$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -664,7 +664,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{7F4E59C2-19AB-F943-BFF6-4A1B45EC2EAF}</c15:txfldGUID>
+                      <c15:txfldGUID>{202157F2-14A6-374A-8578-7704FD57B10F}</c15:txfldGUID>
                       <c15:f>Sheet1!$F$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -704,7 +704,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{2C10629A-00F8-AA4A-94C1-072C8DE08202}</c15:txfldGUID>
+                      <c15:txfldGUID>{CFF96E34-0665-7043-9BE2-F368007B331B}</c15:txfldGUID>
                       <c15:f>Sheet1!$G$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -744,7 +744,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{7BB37772-2767-3A46-A9DF-7B79D0A168F8}</c15:txfldGUID>
+                      <c15:txfldGUID>{2C21E42D-67D4-A447-A330-02FBDA4AA720}</c15:txfldGUID>
                       <c15:f>Sheet1!$H$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -784,7 +784,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{E3300176-1E03-C744-9B10-2E4E7CDE5513}</c15:txfldGUID>
+                      <c15:txfldGUID>{97B2CC3D-0ACC-DD40-AA88-2BF94584C677}</c15:txfldGUID>
                       <c15:f>Sheet1!$I$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -824,7 +824,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{06F5030F-821B-DF4A-B714-C1EF02617C9E}</c15:txfldGUID>
+                      <c15:txfldGUID>{A30F64FB-0090-434F-9B7E-F1E65CFCEEF7}</c15:txfldGUID>
                       <c15:f>Sheet1!$J$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -864,7 +864,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{F711737E-CFE1-9243-9E7A-1DC5219BE02B}</c15:txfldGUID>
+                      <c15:txfldGUID>{26450C7C-232A-BA44-8A09-1256B871BAFD}</c15:txfldGUID>
                       <c15:f>Sheet1!$K$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -904,7 +904,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{A3C137CE-159A-7A4E-832A-AB5CF21FC0A8}</c15:txfldGUID>
+                      <c15:txfldGUID>{D217F776-8448-D940-A81D-11556BD7DBDF}</c15:txfldGUID>
                       <c15:f>Sheet1!$L$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -944,7 +944,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{247357A3-64BD-ED49-A010-8DD2E049313E}</c15:txfldGUID>
+                      <c15:txfldGUID>{8241549B-9173-7E47-A518-4A52F5754F95}</c15:txfldGUID>
                       <c15:f>Sheet1!$M$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -984,7 +984,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{5B158D5E-FCA9-944E-AF16-CBC1CDD8E6B9}</c15:txfldGUID>
+                      <c15:txfldGUID>{004D810A-6317-A14B-B489-A1302A5208F5}</c15:txfldGUID>
                       <c15:f>Sheet1!$N$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -1024,7 +1024,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{C2E35656-593C-DD4F-BF3C-B0BC7E086D53}</c15:txfldGUID>
+                      <c15:txfldGUID>{6D388E2E-9603-234A-BE6F-EC24294A2505}</c15:txfldGUID>
                       <c15:f>Sheet1!$O$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -1652,7 +1652,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{303C924B-75F1-0B4E-B68C-ACD6708DB759}</c15:txfldGUID>
+                      <c15:txfldGUID>{EC25B926-B3D1-7E4C-A7C6-AD1053CAB4D2}</c15:txfldGUID>
                       <c15:f>Sheet1!$B$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -1692,7 +1692,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{E0404777-FC08-974F-B16E-BE27C2213E8C}</c15:txfldGUID>
+                      <c15:txfldGUID>{1E774387-E8F2-C34A-9486-EDE11D4045AA}</c15:txfldGUID>
                       <c15:f>Sheet1!$C$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -1732,7 +1732,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{07302DB1-5E71-D64A-B710-D23FAC32215C}</c15:txfldGUID>
+                      <c15:txfldGUID>{E61EE3B2-54A2-824D-8764-ADAE91F23583}</c15:txfldGUID>
                       <c15:f>Sheet1!$D$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -1772,7 +1772,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{E23EFFE8-249C-614A-B2BD-33D928F191F1}</c15:txfldGUID>
+                      <c15:txfldGUID>{B83E88FE-C0BF-E042-AFE0-F99307E67AA5}</c15:txfldGUID>
                       <c15:f>Sheet1!$E$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -1812,7 +1812,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{B221631E-0721-3B47-B1B1-7E017BEACC61}</c15:txfldGUID>
+                      <c15:txfldGUID>{129ED5BF-7782-BA41-8567-8601FC81EBD3}</c15:txfldGUID>
                       <c15:f>Sheet1!$F$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -1852,7 +1852,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{4633C010-13B3-4C4A-BC0B-5E70D65C6A69}</c15:txfldGUID>
+                      <c15:txfldGUID>{B6B02316-A437-8E49-8B13-77C168862E85}</c15:txfldGUID>
                       <c15:f>Sheet1!$G$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -1892,7 +1892,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{20F24394-CAD7-1844-BCEF-9864448E76F6}</c15:txfldGUID>
+                      <c15:txfldGUID>{6ED214B0-CFC5-7B4A-92B5-24A44558BC0F}</c15:txfldGUID>
                       <c15:f>Sheet1!$H$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -1932,7 +1932,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{C5F546F0-B6E5-4142-8FA2-11E9DE4D8AF2}</c15:txfldGUID>
+                      <c15:txfldGUID>{146A4B75-094D-4545-8838-B4718A8299EA}</c15:txfldGUID>
                       <c15:f>Sheet1!$I$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -1972,7 +1972,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{BC1A3EAC-5051-0440-9F0E-68F0E15E52A7}</c15:txfldGUID>
+                      <c15:txfldGUID>{86FAC3CB-DE40-AE40-8258-518549CC0AFA}</c15:txfldGUID>
                       <c15:f>Sheet1!$J$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -2012,7 +2012,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{F91B8E70-7907-DF41-8477-480CA90A128D}</c15:txfldGUID>
+                      <c15:txfldGUID>{BC9F342C-9D34-514B-AF7E-9F15F93E6D91}</c15:txfldGUID>
                       <c15:f>Sheet1!$K$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -2052,7 +2052,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{9599A410-E20D-F248-8206-AA96398CCFED}</c15:txfldGUID>
+                      <c15:txfldGUID>{95B38563-6773-AC48-B1F2-BBED4458F18C}</c15:txfldGUID>
                       <c15:f>Sheet1!$L$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -2092,7 +2092,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{943A7CE8-AB73-9E48-85F6-FA31233C52AB}</c15:txfldGUID>
+                      <c15:txfldGUID>{45B5BA78-C21D-4C4E-BF7B-7CCE8E01551A}</c15:txfldGUID>
                       <c15:f>Sheet1!$M$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -2132,7 +2132,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{8E56BA54-BB5C-DC4A-A04C-2A7806AF0395}</c15:txfldGUID>
+                      <c15:txfldGUID>{F266A541-DD91-7543-BE92-2E7052A5A883}</c15:txfldGUID>
                       <c15:f>Sheet1!$N$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -2172,7 +2172,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{FD94986B-2546-3C4F-B67B-64E41392A349}</c15:txfldGUID>
+                      <c15:txfldGUID>{C2E28ACE-776E-5848-B5CD-86A3CD0B42BC}</c15:txfldGUID>
                       <c15:f>Sheet1!$O$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -2703,51 +2703,51 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$42:$O$42</c:f>
+              <c:f>Sheet1!$B$41:$O$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>1.31610432E7</c:v>
+                  <c:v>1.38441573333333E7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.68957530666667E7</c:v>
+                  <c:v>1.80708357333333E7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.38715162666667E7</c:v>
+                  <c:v>2.62238464E7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.77897173333333E7</c:v>
+                  <c:v>2.03101168E7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.81777813333333E7</c:v>
+                  <c:v>2.18891029333333E7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.42281253333333E7</c:v>
+                  <c:v>1.91731765333333E7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.89428096E7</c:v>
+                  <c:v>2.24071498666667E7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.44573845333333E7</c:v>
+                  <c:v>1.91403664E7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.72344858666667E7</c:v>
+                  <c:v>2.36933578666667E7</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.16447434666667E7</c:v>
+                  <c:v>1.89485818666667E7</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.45397952E7</c:v>
+                  <c:v>1.69990661333333E7</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.86128864E7</c:v>
+                  <c:v>2.19106448E7</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.27482346666667E7</c:v>
+                  <c:v>2.48818496E7</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.56258218666667E7</c:v>
+                  <c:v>1.76442688E7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2803,7 +2803,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{F2FB49D5-48DD-0C4F-A38E-C1CAB391E303}</c15:txfldGUID>
+                      <c15:txfldGUID>{5C515C88-86AE-D04C-814D-9AD6B8C58872}</c15:txfldGUID>
                       <c15:f>Sheet1!$B$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -2842,7 +2842,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{A01955F5-8850-CE47-962B-1880DA58BC25}</c15:txfldGUID>
+                      <c15:txfldGUID>{264ED0D0-FB64-354C-96B8-F274C65DCD11}</c15:txfldGUID>
                       <c15:f>Sheet1!$C$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -2881,7 +2881,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{6D08502A-64C9-B844-9914-AE0D18DD6315}</c15:txfldGUID>
+                      <c15:txfldGUID>{19D91D8B-15A9-F147-96DC-69E4C6C6232B}</c15:txfldGUID>
                       <c15:f>Sheet1!$D$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -2920,7 +2920,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{B7507227-58B3-7A45-B4AF-6350933610EC}</c15:txfldGUID>
+                      <c15:txfldGUID>{58513C24-4B57-6845-A56C-95A77302D915}</c15:txfldGUID>
                       <c15:f>Sheet1!$E$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -2959,7 +2959,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{26CC366C-7545-1149-B6B5-0F9C8923F93D}</c15:txfldGUID>
+                      <c15:txfldGUID>{EDB1D721-7718-9945-AD7E-48A22D290906}</c15:txfldGUID>
                       <c15:f>Sheet1!$F$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -2998,7 +2998,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{84FE5459-1C11-8F4A-9DEC-CEB8D81ED74C}</c15:txfldGUID>
+                      <c15:txfldGUID>{75D28407-5565-7E46-8E1D-C4368684610F}</c15:txfldGUID>
                       <c15:f>Sheet1!$G$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -3037,7 +3037,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{326B24AE-3CF7-7B4F-8965-FD8CC2803001}</c15:txfldGUID>
+                      <c15:txfldGUID>{EF45E2C2-28CA-504F-A7BE-562E5DF743BC}</c15:txfldGUID>
                       <c15:f>Sheet1!$H$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -3076,7 +3076,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{01AD98EF-4359-D64D-B3E3-F6E9765BF573}</c15:txfldGUID>
+                      <c15:txfldGUID>{3389794E-66BC-E64C-B7A3-C4C7125CCDFC}</c15:txfldGUID>
                       <c15:f>Sheet1!$I$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -3115,7 +3115,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{D7612D7F-A1F8-CD44-9B60-02FBE9ECBE4E}</c15:txfldGUID>
+                      <c15:txfldGUID>{E50AA2D9-7BB5-6B42-97D6-F9969765D1B4}</c15:txfldGUID>
                       <c15:f>Sheet1!$J$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -3154,7 +3154,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{96B5B11E-0DEF-074D-95D3-8B4C93C02417}</c15:txfldGUID>
+                      <c15:txfldGUID>{C4E1E6B1-5808-C647-A71D-D9B64416E275}</c15:txfldGUID>
                       <c15:f>Sheet1!$K$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -3193,7 +3193,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{13AF1B19-F830-B949-A8CA-8B814C14D17F}</c15:txfldGUID>
+                      <c15:txfldGUID>{7B2EF857-D603-3C47-B1A7-9A432907A483}</c15:txfldGUID>
                       <c15:f>Sheet1!$L$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -3232,7 +3232,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{83906C27-637D-CF4D-901D-21AE5AAD29BF}</c15:txfldGUID>
+                      <c15:txfldGUID>{CA9D6E6E-8247-D240-90BE-A801EBE3AD59}</c15:txfldGUID>
                       <c15:f>Sheet1!$M$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -3271,7 +3271,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{AD6D028F-5994-2C4B-BECA-54691D025EF3}</c15:txfldGUID>
+                      <c15:txfldGUID>{3D600841-C644-3F4F-9F64-37835467DE8D}</c15:txfldGUID>
                       <c15:f>Sheet1!$N$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -3310,7 +3310,7 @@
                   <c15:layout/>
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{86BA1A02-13BA-C345-8EF9-5DC1B0FFA1DE}</c15:txfldGUID>
+                      <c15:txfldGUID>{F87D4A5E-2B8D-B14E-8EB2-E2D808B3F41D}</c15:txfldGUID>
                       <c15:f>Sheet1!$O$5</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5459,13 +5459,13 @@
       <xdr:col>11</xdr:col>
       <xdr:colOff>14768</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>29536</xdr:rowOff>
+      <xdr:rowOff>29537</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>177209</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>118141</xdr:rowOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7837,7 +7837,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J8" zoomScale="86" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G9" zoomScale="86" workbookViewId="0">
       <selection activeCell="Y33" sqref="Y33"/>
     </sheetView>
   </sheetViews>

</xml_diff>